<commit_message>
Clean up from 102317
Good basis of glm, need some wing stuff
</commit_message>
<xml_diff>
--- a/lifehist/2017_10_21 Life history stats resutls.xlsx
+++ b/lifehist/2017_10_21 Life history stats resutls.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21765" windowHeight="10245" firstSheet="4" activeTab="9"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21765" windowHeight="10245" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="GLMAdrate and all data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="Emergence time" sheetId="7" r:id="rId7"/>
     <sheet name="AdRate" sheetId="8" r:id="rId8"/>
     <sheet name="LarvRate" sheetId="9" r:id="rId9"/>
-    <sheet name="length of adult life" sheetId="10" r:id="rId10"/>
+    <sheet name="Wing size" sheetId="11" r:id="rId10"/>
+    <sheet name="length of adult life" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="995">
   <si>
     <t>GLM building for rate of development</t>
   </si>
@@ -2543,6 +2544,503 @@
   </si>
   <si>
     <t xml:space="preserve"> 3         A        F   5.196970 0.09802522 2634 5.004755 5.389184            A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coxph(formula = Surv(time, Death_stat) ~ Lat_group + Temp_let + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Sex, data = survive)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              coef exp(coef) se(coef)      z      p</t>
+  </si>
+  <si>
+    <t>Lat_group2 -1.0243    0.3591   0.0448 -22.87 &lt;2e-16</t>
+  </si>
+  <si>
+    <t>Lat_group3 -1.8181    0.1623   0.0744 -24.42 &lt;2e-16</t>
+  </si>
+  <si>
+    <t>Temp_letB   1.5671    4.7926   0.0524  29.89 &lt;2e-16</t>
+  </si>
+  <si>
+    <t>Temp_letC   2.5956   13.4051   0.0614  42.30 &lt;2e-16</t>
+  </si>
+  <si>
+    <t>SexF       -0.0995    0.9053   0.0391  -2.55  0.011</t>
+  </si>
+  <si>
+    <t>SexM            NA        NA   0.0000     NA     NA</t>
+  </si>
+  <si>
+    <t>Likelihood ratio test=2374  on 5 df, p=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n= 2652, number of events= 2652 </t>
+  </si>
+  <si>
+    <t>&gt; resall1.cox&lt;- coxph(Surv(time, Death_stat)~Lat_group*Temp_let*Sex,data=survive)</t>
+  </si>
+  <si>
+    <r>
+      <t>X matrix deemed to be singular; variable 6 13 14 17 18 23 24 25 26</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt; resall1.cox</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">coxph(formula = Surv(time, Death_stat) ~ Lat_group * Temp_let * </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                             coef exp(coef) se(coef)      z      p</t>
+  </si>
+  <si>
+    <t>Lat_group2                -0.8981    0.4073   0.1001  -8.98 &lt;2e-16</t>
+  </si>
+  <si>
+    <t>Lat_group3                -1.6999    0.1827   0.1510 -11.26 &lt;2e-16</t>
+  </si>
+  <si>
+    <t>Temp_letB                  1.5544    4.7324   0.1092  14.23 &lt;2e-16</t>
+  </si>
+  <si>
+    <t>Temp_letC                  2.8620   17.4964   0.1155  24.77 &lt;2e-16</t>
+  </si>
+  <si>
+    <t>SexF                       0.0814    1.0848   0.1104   0.74 0.4608</t>
+  </si>
+  <si>
+    <t>SexM                           NA        NA   0.0000     NA     NA</t>
+  </si>
+  <si>
+    <t>Lat_group2:Temp_letB       0.0522    1.0536   0.1403   0.37 0.7098</t>
+  </si>
+  <si>
+    <t>Lat_group3:Temp_letB       0.1101    1.1164   0.2079   0.53 0.5965</t>
+  </si>
+  <si>
+    <t>Lat_group2:Temp_letC      -0.3391    0.7124   0.1453  -2.33 0.0197</t>
+  </si>
+  <si>
+    <t>Lat_group3:Temp_letC      -0.7037    0.4948   0.2972  -2.37 0.0179</t>
+  </si>
+  <si>
+    <t>Lat_group2:SexF           -0.1918    0.8255   0.1427  -1.34 0.1788</t>
+  </si>
+  <si>
+    <t>Lat_group3:SexF           -0.3660    0.6935   0.2097  -1.75 0.0809</t>
+  </si>
+  <si>
+    <t>Lat_group2:SexM                NA        NA   0.0000     NA     NA</t>
+  </si>
+  <si>
+    <t>Lat_group3:SexM                NA        NA   0.0000     NA     NA</t>
+  </si>
+  <si>
+    <t>Temp_letB:SexF            -0.1918    0.8254   0.1557  -1.23 0.2178</t>
+  </si>
+  <si>
+    <t>Temp_letC:SexF            -0.1426    0.8671   0.1590  -0.90 0.3695</t>
+  </si>
+  <si>
+    <t>Temp_letB:SexM                 NA        NA   0.0000     NA     NA</t>
+  </si>
+  <si>
+    <t>Temp_letC:SexM                 NA        NA   0.0000     NA     NA</t>
+  </si>
+  <si>
+    <t>Lat_group2:Temp_letB:SexF  0.1817    1.1992   0.2010   0.90 0.3661</t>
+  </si>
+  <si>
+    <t>Lat_group3:Temp_letB:SexF  0.3401    1.4051   0.2981   1.14 0.2540</t>
+  </si>
+  <si>
+    <t>Lat_group2:Temp_letC:SexF  0.0342    1.0348   0.2089   0.16 0.8698</t>
+  </si>
+  <si>
+    <t>Lat_group3:Temp_letC:SexF  1.1463    3.1465   0.4230   2.71 0.0067</t>
+  </si>
+  <si>
+    <t>Lat_group2:Temp_letB:SexM      NA        NA   0.0000     NA     NA</t>
+  </si>
+  <si>
+    <t>Lat_group3:Temp_letB:SexM      NA        NA   0.0000     NA     NA</t>
+  </si>
+  <si>
+    <t>Lat_group2:Temp_letC:SexM      NA        NA   0.0000     NA     NA</t>
+  </si>
+  <si>
+    <t>Lat_group3:Temp_letC:SexM      NA        NA   0.0000     NA     NA</t>
+  </si>
+  <si>
+    <t>Likelihood ratio test=2407  on 17 df, p=0</t>
+  </si>
+  <si>
+    <t>summary(al_fit5p)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Family: poisson  ( log )</t>
+  </si>
+  <si>
+    <t>Formula: AL ~ (1 | Biome) + Lat_group + Temp_let + Sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  8366.3   8407.4  -4176.1   8352.3     2645 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Min       1Q   Median       3Q      Max </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2.10676 -0.20811  0.05416  0.22407  1.69054 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Groups Name        Variance Std.Dev.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Biome  (Intercept) 0.002417 0.04916 </t>
+  </si>
+  <si>
+    <t>Number of obs: 2652, groups:  Biome, 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Estimate Std. Error z value Pr(&gt;|z|)    </t>
+  </si>
+  <si>
+    <t>(Intercept)  1.52775    0.04719   32.38  &lt; 2e-16 ***</t>
+  </si>
+  <si>
+    <t>Lat_group2  -0.10459    0.02558   -4.09 4.34e-05 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group3   0.01848    0.07347    0.25    0.801    </t>
+  </si>
+  <si>
+    <t>Temp_letB   -0.43985    0.02482  -17.72  &lt; 2e-16 ***</t>
+  </si>
+  <si>
+    <t>Temp_letC   -0.83545    0.03122  -26.76  &lt; 2e-16 ***</t>
+  </si>
+  <si>
+    <t>SexM        -0.09061    0.02211   -4.10 4.18e-05 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           (Intr) Lt_gr2 Lt_gr3 Tmp_lB Tmp_lC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group2 -0.439                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group3 -0.577  0.276                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temp_letB  -0.201 -0.004  0.001              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temp_letC  -0.173  0.023  0.050  0.312       </t>
+  </si>
+  <si>
+    <t>SexM       -0.246  0.039  0.014 -0.006 -0.022</t>
+  </si>
+  <si>
+    <t>wl_fit1b&lt;-glmer(Wing.length..mm.~(1|Biome)+(1|State), data=survive, family=Gamma)</t>
+  </si>
+  <si>
+    <t>&gt; summary(wl_fit7b)</t>
+  </si>
+  <si>
+    <t>Formula: Wing.length..mm. ~ (1 | Biome) + (1 | State) + Lat_group * Temp_let *      Sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -3380.0  -3257.1   1711.0  -3422.0     2558 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3.3355 -0.6859 -0.0575  0.6187  3.6953 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Groups   Name        Variance  Std.Dev. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> State    (Intercept) 1.251e-11 3.537e-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Biome    (Intercept) 1.663e-06 1.290e-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Residual             2.174e-03 4.663e-02</t>
+  </si>
+  <si>
+    <t>Number of obs: 2579, groups:  State, 4; Biome, 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                            Estimate Std. Error t value Pr(&gt;|z|)    </t>
+  </si>
+  <si>
+    <t>(Intercept)                0.3607235  0.0027653  130.45  &lt; 2e-16 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group2                -0.0041769  0.0017646   -2.37 0.017932 *  </t>
+  </si>
+  <si>
+    <t>Lat_group3                -0.0295570  0.0041794   -7.07 1.53e-12 ***</t>
+  </si>
+  <si>
+    <t>Temp_letB                  0.0234090  0.0020075   11.66  &lt; 2e-16 ***</t>
+  </si>
+  <si>
+    <t>Temp_letC                  0.0358522  0.0021048   17.03  &lt; 2e-16 ***</t>
+  </si>
+  <si>
+    <t>SexM                      -0.0063371  0.0018835   -3.36 0.000767 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group2:Temp_letB      -0.0029579  0.0025396   -1.16 0.244141    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group3:Temp_letB       0.0064814  0.0035787    1.81 0.070123 .  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group2:Temp_letC       0.0059529  0.0027402    2.17 0.029822 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group3:Temp_letC       0.0134563  0.0052584    2.56 0.010497 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group2:SexM            0.0007504  0.0024111    0.31 0.755614    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group3:SexM            0.0109664  0.0033364    3.29 0.001013 ** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temp_letB:SexM            -0.0020997  0.0027458   -0.76 0.444451    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temp_letC:SexM            -0.0058098  0.0028352   -2.05 0.040444 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group2:Temp_letB:SexM -0.0022100  0.0035094   -0.63 0.528863    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group3:Temp_letB:SexM -0.0031888  0.0049709   -0.64 0.521202    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group2:Temp_letC:SexM  0.0008759  0.0037240    0.24 0.814054    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group3:Temp_letC:SexM -0.0038803  0.0072888   -0.53 0.594471    </t>
+  </si>
+  <si>
+    <t>Correlation matrix not shown by default, as p = 18 &gt; 12.</t>
+  </si>
+  <si>
+    <t>Use print(x, correlation=TRUE)  or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         vcov(x)         if you need it</t>
+  </si>
+  <si>
+    <t>convergence code: 0</t>
+  </si>
+  <si>
+    <t>Model failed to converge with max|grad| = 0.0153395 (tol = 0.001, component 1)</t>
+  </si>
+  <si>
+    <t>Model is nearly unidentifiable: very large eigenvalue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Rescale variables?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> wl_anca&lt;-lm(Wing.length..mm.~Lat_group*Temp_let, data=survive)</t>
+  </si>
+  <si>
+    <t>&gt; summary(wl_anca)</t>
+  </si>
+  <si>
+    <t>lm(formula = Wing.length..mm. ~ Lat_group * Temp_let, data = survive)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.42387 -0.08623 -0.00509  0.08113  0.42878 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                      Estimate Std. Error t value Pr(&gt;|t|)    </t>
+  </si>
+  <si>
+    <t>(Intercept)           2.764093   0.007190 384.454  &lt; 2e-16 ***</t>
+  </si>
+  <si>
+    <t>Lat_group2            0.038773   0.009265   4.185 2.95e-05 ***</t>
+  </si>
+  <si>
+    <t>Lat_group3            0.235237   0.013503  17.421  &lt; 2e-16 ***</t>
+  </si>
+  <si>
+    <t>Temp_letB            -0.160860   0.010168 -15.821  &lt; 2e-16 ***</t>
+  </si>
+  <si>
+    <t>Temp_letC            -0.227872   0.010309 -22.104  &lt; 2e-16 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group2:Temp_letB  0.024366   0.013105   1.859 0.063101 .  </t>
+  </si>
+  <si>
+    <t>Lat_group3:Temp_letB -0.066056   0.019356  -3.413 0.000653 ***</t>
+  </si>
+  <si>
+    <t>Lat_group2:Temp_letC -0.047676   0.013551  -3.518 0.000442 ***</t>
+  </si>
+  <si>
+    <t>Lat_group3:Temp_letC -0.124883   0.027198  -4.592 4.61e-06 ***</t>
+  </si>
+  <si>
+    <t>Residual standard error: 0.1288 on 2570 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (73 observations deleted due to missingness)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple R-squared:  0.489,     Adjusted R-squared:  0.4875 </t>
+  </si>
+  <si>
+    <t>F-statistic: 307.5 on 8 and 2570 DF,  p-value: &lt; 2.2e-16</t>
+  </si>
+  <si>
+    <t>&gt; al_anclsa&lt;-cld(lsmeans(wl_anca, c("Lat_group", "Temp_let")))</t>
+  </si>
+  <si>
+    <t>&gt; al_anclsa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lat_group Temp_let   lsmean          SE   df lower.CL upper.CL .group </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2         C        2.527319 0.006573477 2570 2.514429 2.540209  1     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1         C        2.536221 0.007387950 2570 2.521734 2.550708  1     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1         B        2.603234 0.007189658 2570 2.589136 2.617332   2    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3         C        2.646576 0.022423519 2570 2.602606 2.690546   23   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2         B        2.666373 0.005849111 2570 2.654903 2.677842    3   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1         A        2.764093 0.007189658 2570 2.749995 2.778192     4  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3         B        2.772415 0.011858227 2570 2.749163 2.795668     45 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2         A        2.802867 0.005843090 2570 2.791409 2.814324      5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3         A        2.999331 0.011430333 2570 2.976917 3.021744       6</t>
+  </si>
+  <si>
+    <t>summary(glmer(LarvRate~(1|Biome)+(1|State)+Lat_group*Temp_let, data=survive, family=Gamma))</t>
+  </si>
+  <si>
+    <t>Formula: LarvRate ~ (1 | Biome) + (1 | State) + Lat_group * Temp_let</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-18536.8 -18466.2   9280.4 -18560.8     2640 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2.7466 -0.6880 -0.1983  0.5577  4.1085 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Groups   Name        Variance  Std.Dev.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> State    (Intercept) 0.0002537 0.01593 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Biome    (Intercept) 0.0713834 0.26718 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Residual             0.0166674 0.12910 </t>
+  </si>
+  <si>
+    <t>Number of obs: 2652, groups:  State, 4; Biome, 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     Estimate Std. Error t value Pr(&gt;|z|)    </t>
+  </si>
+  <si>
+    <t>(Intercept)           19.4887     0.5866   33.22  &lt; 2e-16 ***</t>
+  </si>
+  <si>
+    <t>Lat_group2             2.1446     0.1790   11.98  &lt; 2e-16 ***</t>
+  </si>
+  <si>
+    <t>Lat_group3             3.7857     0.8606    4.40 1.09e-05 ***</t>
+  </si>
+  <si>
+    <t>Temp_letB             -2.6481     0.1666  -15.90  &lt; 2e-16 ***</t>
+  </si>
+  <si>
+    <t>Temp_letC             -4.6891     0.1599  -29.32  &lt; 2e-16 ***</t>
+  </si>
+  <si>
+    <t>Lat_group2:Temp_letB  -0.7480     0.2265   -3.30 0.000957 ***</t>
+  </si>
+  <si>
+    <t>Lat_group3:Temp_letB  -1.7521     0.3766   -4.65 3.28e-06 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group2:Temp_letC  -0.3748     0.2223   -1.69 0.091789 .  </t>
+  </si>
+  <si>
+    <t>Lat_group3:Temp_letC  -2.4419     0.4690   -5.21 1.92e-07 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            (Intr) Lt_gr2 Lt_gr3 Tmp_lB Tmp_lC L_2:T_B L_3:T_B L_2:T_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group2  -0.199                                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lat_group3  -0.679  0.135                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temp_letB   -0.164  0.538  0.111                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temp_letC   -0.171  0.561  0.116  0.603                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lt_grp2:T_B  0.123 -0.741 -0.084 -0.735 -0.443                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lt_grp3:T_B  0.071 -0.238 -0.256 -0.442 -0.266  0.325                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lt_grp2:T_C  0.126 -0.755 -0.086 -0.434 -0.719  0.595   0.191         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lt_grp3:T_C  0.057 -0.191 -0.205 -0.205 -0.340  0.151   0.472   0.245 </t>
+  </si>
+  <si>
+    <t>Model failed to converge with max|grad| = 0.355353 (tol = 0.001, component 1)</t>
+  </si>
+  <si>
+    <t>Warning message:</t>
+  </si>
+  <si>
+    <t>In checkConv(attr(opt, "derivs"), opt$par, ctrl = control$checkConv,  :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Model failed to converge with max|grad| = 0.355353 (tol = 0.001, component 1)</t>
   </si>
 </sst>
 </file>
@@ -2840,10 +3338,17 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2864,18 +3369,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3205,7 +3703,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="56"/>
+      <c r="B3" s="59"/>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3213,11 +3711,11 @@
         <v>3</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="57"/>
+      <c r="B4" s="60"/>
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
@@ -3225,8 +3723,8 @@
         <v>2</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
@@ -3360,9 +3858,9 @@
       <c r="C17" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="54"/>
+      <c r="D17" s="57"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="54"/>
+      <c r="F17" s="57"/>
       <c r="G17" s="8" t="s">
         <v>36</v>
       </c>
@@ -3374,9 +3872,9 @@
       <c r="C18" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="54"/>
+      <c r="D18" s="57"/>
       <c r="E18" s="14"/>
-      <c r="F18" s="54"/>
+      <c r="F18" s="57"/>
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3384,9 +3882,9 @@
         <v>2</v>
       </c>
       <c r="C19" s="13"/>
-      <c r="D19" s="55"/>
+      <c r="D19" s="58"/>
       <c r="E19" s="19"/>
-      <c r="F19" s="55"/>
+      <c r="F19" s="58"/>
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
@@ -3528,7 +4026,7 @@
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="60"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="10" t="s">
         <v>1</v>
       </c>
@@ -3536,11 +4034,11 @@
         <v>3</v>
       </c>
       <c r="E32" s="10"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
     </row>
     <row r="33" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="61"/>
+      <c r="B33" s="56"/>
       <c r="C33" s="12" t="s">
         <v>2</v>
       </c>
@@ -3548,8 +4046,8 @@
         <v>2</v>
       </c>
       <c r="E33" s="12"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="55"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="22" t="s">
@@ -3690,26 +4188,26 @@
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="52"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E46" s="54"/>
-      <c r="F46" s="54"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="53"/>
+      <c r="B47" s="64"/>
       <c r="C47" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D47" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E47" s="55"/>
-      <c r="F47" s="55"/>
+      <c r="E47" s="58"/>
+      <c r="F47" s="58"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="16" t="s">
@@ -3832,29 +4330,29 @@
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="56"/>
+      <c r="B60" s="59"/>
       <c r="C60" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E60" s="58"/>
-      <c r="F60" s="58"/>
+      <c r="E60" s="61"/>
+      <c r="F60" s="61"/>
       <c r="G60" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="61" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="57"/>
+      <c r="B61" s="60"/>
       <c r="C61" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E61" s="59"/>
-      <c r="F61" s="59"/>
+      <c r="E61" s="62"/>
+      <c r="F61" s="62"/>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
@@ -3977,6 +4475,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="F32:F33"/>
     <mergeCell ref="G32:G33"/>
@@ -3985,12 +4489,6 @@
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="D17:D19"/>
     <mergeCell ref="F17:F19"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="F60:F61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3999,319 +4497,813 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L106"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:A106"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>898</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>547</v>
+      </c>
+      <c r="M3" s="42" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>548</v>
+      </c>
+      <c r="M4" s="26"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>899</v>
+      </c>
+      <c r="M5" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>550</v>
+      </c>
+      <c r="M6" s="27" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="26"/>
+      <c r="M7" s="26"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>551</v>
+      </c>
+      <c r="M8" s="27" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>900</v>
+      </c>
+      <c r="M9" s="27" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
+      <c r="M10" s="27" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>553</v>
+      </c>
+      <c r="M11" s="26"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>554</v>
+      </c>
+      <c r="M12" s="27" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>901</v>
+      </c>
+      <c r="M13" s="27" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="26"/>
+      <c r="M14" s="27" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
+        <v>556</v>
+      </c>
+      <c r="M15" s="27" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
+        <v>902</v>
+      </c>
+      <c r="M16" s="27" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>903</v>
+      </c>
+      <c r="M17" s="27" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>904</v>
+      </c>
+      <c r="M18" s="27" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>905</v>
+      </c>
+      <c r="M19" s="27" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>906</v>
+      </c>
+      <c r="M20" s="27" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="26"/>
+      <c r="M21" s="27" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>562</v>
+      </c>
+      <c r="M22" s="27" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>907</v>
+      </c>
+      <c r="M23" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>908</v>
+      </c>
+      <c r="M24" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
+        <v>909</v>
+      </c>
+      <c r="M25" s="26"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
+        <v>910</v>
+      </c>
+      <c r="M26" s="27" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
+        <v>911</v>
+      </c>
+      <c r="M27" s="27" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
+        <v>912</v>
+      </c>
+      <c r="M28" s="27" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
+        <v>913</v>
+      </c>
+      <c r="M29" s="27" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="27" t="s">
+        <v>914</v>
+      </c>
+      <c r="M30" s="26"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
+        <v>915</v>
+      </c>
+      <c r="M31" s="42" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="27" t="s">
+        <v>916</v>
+      </c>
+      <c r="M32" s="42" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="27" t="s">
+        <v>917</v>
+      </c>
+      <c r="M33" s="27" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
+        <v>918</v>
+      </c>
+      <c r="M34" s="27" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
+        <v>919</v>
+      </c>
+      <c r="M35" s="27" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
+        <v>920</v>
+      </c>
+      <c r="M36" s="27" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>921</v>
+      </c>
+      <c r="M37" s="27" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
+        <v>922</v>
+      </c>
+      <c r="M38" s="27" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="27" t="s">
+        <v>923</v>
+      </c>
+      <c r="M39" s="27" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="27" t="s">
+        <v>924</v>
+      </c>
+      <c r="M40" s="27" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="27" t="s">
+        <v>925</v>
+      </c>
+      <c r="M41" s="27" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="M42" s="27" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M43" s="26"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="26"/>
+      <c r="M44" s="27" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="43" t="s">
+        <v>926</v>
+      </c>
+      <c r="M45" s="27" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="43" t="s">
+        <v>927</v>
+      </c>
+      <c r="M46" s="27" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="43" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="26"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="27" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="27" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="27" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="27" t="s">
+        <v>932</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U106"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y26" sqref="Y26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>702</v>
       </c>
       <c r="K1" s="25" t="s">
         <v>731</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U1" s="25" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>703</v>
       </c>
       <c r="K2" s="42" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U2" s="27" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
       <c r="K3" s="26"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U3" s="27" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>54</v>
       </c>
       <c r="K4" s="27" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U4" s="27" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>704</v>
       </c>
       <c r="K5" s="27" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U5" s="27" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="26"/>
       <c r="K6" s="26"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U6" s="26"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>451</v>
       </c>
       <c r="K7" s="27" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U7" s="27" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
         <v>554</v>
       </c>
       <c r="K8" s="27" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U8" s="27" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
         <v>705</v>
       </c>
       <c r="K9" s="27" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U9" s="26"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="K10" s="26"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U10" s="27" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>454</v>
       </c>
       <c r="K11" s="27" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U11" s="27" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
         <v>706</v>
       </c>
       <c r="K12" s="27" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U12" s="27" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
         <v>707</v>
       </c>
       <c r="K13" s="27" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U13" s="26"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
         <v>708</v>
       </c>
       <c r="K14" s="27" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U14" s="27" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>709</v>
       </c>
       <c r="K15" s="27" t="s">
         <v>737</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U15" s="27" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>710</v>
       </c>
       <c r="K16" s="27" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U16" s="27" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>711</v>
       </c>
       <c r="K17" s="27" t="s">
         <v>739</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U17" s="27" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>712</v>
       </c>
       <c r="K18" s="27" t="s">
         <v>740</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U18" s="26"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>713</v>
       </c>
       <c r="K19" s="27" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U19" s="27" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>714</v>
       </c>
       <c r="K20" s="27" t="s">
         <v>742</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U20" s="27" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>715</v>
       </c>
       <c r="K21" s="27" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U21" s="27" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
         <v>55</v>
       </c>
       <c r="K22" s="27" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U22" s="27" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>56</v>
       </c>
       <c r="K23" s="27" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U23" s="27" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
       <c r="K24" s="26"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U24" s="27" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
         <v>716</v>
       </c>
       <c r="K25" s="27" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U25" s="27" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>717</v>
       </c>
       <c r="K26" s="27" t="s">
         <v>745</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U26" s="27" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>718</v>
       </c>
       <c r="K27" s="27" t="s">
         <v>746</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U27" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
       <c r="K28" s="26"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U28" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="42" t="s">
         <v>719</v>
       </c>
       <c r="K29" s="42" t="s">
         <v>747</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U29" s="26"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
         <v>720</v>
       </c>
       <c r="K30" s="42" t="s">
         <v>748</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U30" s="27" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
         <v>721</v>
       </c>
+      <c r="I31" s="53"/>
       <c r="K31" s="27" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="U31" s="27" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
         <v>722</v>
       </c>
+      <c r="I32" s="53"/>
       <c r="K32" s="27" t="s">
         <v>749</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U32" s="27" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>723</v>
       </c>
+      <c r="I33" s="53"/>
       <c r="K33" s="27" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U33" s="27" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
         <v>724</v>
       </c>
+      <c r="I34" s="53"/>
       <c r="K34" s="27" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U34" s="27" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
         <v>725</v>
       </c>
+      <c r="I35" s="53"/>
       <c r="K35" s="27" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U35" s="27" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
         <v>726</v>
       </c>
+      <c r="I36" s="53"/>
       <c r="K36" s="27" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U36" s="27" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
         <v>727</v>
       </c>
+      <c r="I37" s="53"/>
       <c r="K37" s="27" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>728</v>
       </c>
+      <c r="I38" s="53"/>
       <c r="K38" s="27" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
         <v>729</v>
       </c>
+      <c r="I39" s="53"/>
       <c r="K39" s="27" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
         <v>730</v>
       </c>
+      <c r="I40" s="53"/>
       <c r="K40" s="27" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="26"/>
       <c r="K41" s="26"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
         <v>388</v>
       </c>
@@ -4319,12 +5311,12 @@
         <v>388</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
         <v>390</v>
       </c>
@@ -4332,15 +5324,15 @@
         <v>758</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L45" s="42" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L46" s="26"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="25" t="s">
         <v>786</v>
       </c>
@@ -4348,7 +5340,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="42" t="s">
         <v>787</v>
       </c>
@@ -4896,8 +5888,8 @@
       <c r="C17" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54" t="s">
+      <c r="D17" s="57"/>
+      <c r="E17" s="57" t="s">
         <v>111</v>
       </c>
       <c r="F17" s="8"/>
@@ -4909,8 +5901,8 @@
       <c r="C18" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4918,8 +5910,8 @@
         <v>2</v>
       </c>
       <c r="C19" s="13"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -6373,10 +7365,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="L14" sqref="L14:L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6384,12 +7376,12 @@
     <col min="1" max="1" width="82.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>299</v>
       </c>
@@ -6397,7 +7389,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>54</v>
       </c>
@@ -6405,7 +7397,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>300</v>
       </c>
@@ -6413,19 +7405,19 @@
         <v>307</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="26"/>
       <c r="C5" s="48" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>301</v>
       </c>
       <c r="C6" s="15"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>302</v>
       </c>
@@ -6433,7 +7425,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
         <v>303</v>
       </c>
@@ -6441,13 +7433,13 @@
         <v>309</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="26"/>
       <c r="C9" s="48" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>304</v>
       </c>
@@ -6455,7 +7447,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>305</v>
       </c>
@@ -6463,157 +7455,339 @@
         <v>312</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="15"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="48" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>315</v>
       </c>
       <c r="C14" s="48" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L14" s="51" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>54</v>
       </c>
       <c r="C15" s="49"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L15" s="51" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>316</v>
       </c>
       <c r="C16" s="50" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L16" s="51" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L17" s="24"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L18" s="51" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L19" s="51" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L20" s="51" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L21" s="51" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L22" s="51" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L23" s="51" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="42" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L24" s="51" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L25" s="24"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L26" s="51" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L27" s="51" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L28" s="25" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L29" s="43" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L30" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="26"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L31" s="27" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L32" s="27" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L33" s="26"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="42" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L34" s="27" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L35" s="27" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L36" s="27" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="26"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L37" s="27" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L38" s="27" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L39" s="27" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L40" s="27" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="26"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L41" s="27" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L42" s="27" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
         <v>332</v>
+      </c>
+      <c r="L43" s="27" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L44" s="27" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L45" s="27" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L46" s="27" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L47" s="27" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L48" s="27" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="49" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L49" s="27" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="50" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L50" s="27" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="51" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L51" s="27" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="52" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L52" s="27" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="53" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L53" s="27" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="54" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L54" s="27" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="55" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L55" s="27" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="56" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L56" s="27" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="57" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L57" s="27" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="58" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L58" s="27" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="59" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L59" s="27" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="60" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L60" s="27" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="61" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L61" s="26"/>
+    </row>
+    <row r="62" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L62" s="27" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="63" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L63" s="27" t="s">
+        <v>843</v>
       </c>
     </row>
   </sheetData>
@@ -7344,21 +8518,21 @@
       <c r="A2" s="27" t="s">
         <v>438</v>
       </c>
-      <c r="S2" s="62" t="s">
+      <c r="S2" s="52" t="s">
         <v>546</v>
       </c>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>439</v>
       </c>
-      <c r="S3" s="64" t="s">
+      <c r="S3" s="54" t="s">
         <v>547</v>
       </c>
-      <c r="T3" s="63"/>
-      <c r="U3" s="63"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
@@ -8115,369 +9289,507 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L109"/>
+  <dimension ref="A1:V109"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:A109"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>575</v>
       </c>
       <c r="L1" s="25" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V1" s="52" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>576</v>
       </c>
       <c r="L2" s="42" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V2" s="27" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
       <c r="L3" s="26"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V3" s="27" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>54</v>
       </c>
       <c r="L4" s="27" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V4" s="27" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>577</v>
       </c>
       <c r="L5" s="27" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V5" s="27" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="26"/>
       <c r="L6" s="26"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V6" s="26"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>451</v>
       </c>
       <c r="L7" s="27" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V7" s="27" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
         <v>452</v>
       </c>
       <c r="L8" s="27" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V8" s="27" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
         <v>578</v>
       </c>
       <c r="L9" s="27" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V9" s="26"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="L10" s="26"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V10" s="27" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>454</v>
       </c>
       <c r="L11" s="27" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V11" s="27" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
         <v>455</v>
       </c>
       <c r="L12" s="27" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V12" s="27" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
         <v>579</v>
       </c>
       <c r="L13" s="27" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V13" s="26"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
         <v>580</v>
       </c>
       <c r="L14" s="27" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V14" s="27" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>581</v>
       </c>
       <c r="L15" s="27" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V15" s="27" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>582</v>
       </c>
       <c r="L16" s="27" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V16" s="27" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>583</v>
       </c>
       <c r="L17" s="27" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V17" s="27" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>584</v>
       </c>
       <c r="L18" s="27" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V18" s="27" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>585</v>
       </c>
       <c r="L19" s="27" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V19" s="27" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>586</v>
       </c>
       <c r="L20" s="27" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V20" s="26"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>587</v>
       </c>
       <c r="L21" s="27" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V21" s="27" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
         <v>55</v>
       </c>
       <c r="L22" s="27" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V22" s="27" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L23" s="27" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V23" s="27" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
       <c r="L24" s="26"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V24" s="27" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
         <v>588</v>
       </c>
       <c r="L25" s="27" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V25" s="27" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>589</v>
       </c>
       <c r="L26" s="27" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V26" s="27" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>590</v>
       </c>
       <c r="L27" s="27" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V27" s="27" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
       <c r="L28" s="26"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V28" s="27" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="42" t="s">
         <v>591</v>
       </c>
       <c r="L29" s="42" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V29" s="27" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
         <v>335</v>
       </c>
       <c r="L30" s="42" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V30" s="27" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
         <v>592</v>
       </c>
       <c r="L31" s="27" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V31" s="27" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
         <v>489</v>
       </c>
       <c r="L32" s="27" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V32" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>593</v>
       </c>
       <c r="L33" s="27" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V33" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
         <v>594</v>
       </c>
       <c r="L34" s="27" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V34" s="26"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
         <v>595</v>
       </c>
       <c r="L35" s="27" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V35" s="27" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
         <v>596</v>
       </c>
       <c r="L36" s="27" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V36" s="27" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
         <v>597</v>
       </c>
       <c r="L37" s="27" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V37" s="27" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>598</v>
       </c>
       <c r="L38" s="27" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V38" s="27" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
         <v>599</v>
       </c>
       <c r="L39" s="27" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V39" s="27" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
         <v>600</v>
       </c>
       <c r="L40" s="27" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V40" s="27" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
         <v>601</v>
       </c>
       <c r="L41" s="26"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V41" s="27" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="26"/>
       <c r="L42" s="27" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V42" s="27" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V43" s="27" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V44" s="27" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
         <v>390</v>
       </c>
       <c r="L45" s="25" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V45" s="27" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="L46" s="42" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V46" s="27" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="L47" s="26"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V47" s="26"/>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="L48" s="27" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V48" s="43" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="L49" s="27" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V49" s="43" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
         <v>656</v>
       </c>
       <c r="L50" s="26"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="V50" s="43" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="42" t="s">
         <v>657</v>
       </c>
@@ -8485,13 +9797,13 @@
         <v>451</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="26"/>
       <c r="L52" s="27" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="27" t="s">
         <v>54</v>
       </c>
@@ -8499,19 +9811,19 @@
         <v>632</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="27" t="s">
         <v>658</v>
       </c>
       <c r="L54" s="26"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="26"/>
       <c r="L55" s="27" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="27" t="s">
         <v>451</v>
       </c>
@@ -8519,7 +9831,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="27" t="s">
         <v>452</v>
       </c>
@@ -8527,7 +9839,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="27" t="s">
         <v>659</v>
       </c>
@@ -8535,13 +9847,13 @@
         <v>634</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="26"/>
       <c r="L59" s="27" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="27" t="s">
         <v>454</v>
       </c>
@@ -8549,7 +9861,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="27" t="s">
         <v>503</v>
       </c>
@@ -8557,7 +9869,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="27" t="s">
         <v>660</v>
       </c>
@@ -8565,7 +9877,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="27" t="s">
         <v>661</v>
       </c>
@@ -8573,7 +9885,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="27" t="s">
         <v>662</v>
       </c>

</xml_diff>

<commit_message>
Finished draft1 of ASTMH poster
Sent to Jan, await feedback
</commit_message>
<xml_diff>
--- a/lifehist/2017_10_21 Life history stats resutls.xlsx
+++ b/lifehist/2017_10_21 Life history stats resutls.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21765" windowHeight="10245" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21765" windowHeight="10245" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="GLMAdrate and all data" sheetId="1" r:id="rId1"/>
@@ -3345,10 +3345,10 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3369,10 +3369,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4026,7 +4026,7 @@
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="55"/>
+      <c r="B32" s="63"/>
       <c r="C32" s="10" t="s">
         <v>1</v>
       </c>
@@ -4038,7 +4038,7 @@
       <c r="G32" s="57"/>
     </row>
     <row r="33" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="56"/>
+      <c r="B33" s="64"/>
       <c r="C33" s="12" t="s">
         <v>2</v>
       </c>
@@ -4188,7 +4188,7 @@
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="63"/>
+      <c r="B46" s="55"/>
       <c r="C46" s="10" t="s">
         <v>1</v>
       </c>
@@ -4199,7 +4199,7 @@
       <c r="F46" s="57"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="64"/>
+      <c r="B47" s="56"/>
       <c r="C47" s="12" t="s">
         <v>2</v>
       </c>
@@ -4475,12 +4475,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="F60:F61"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="F32:F33"/>
     <mergeCell ref="G32:G33"/>
@@ -4489,6 +4483,12 @@
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="D17:D19"/>
     <mergeCell ref="F17:F19"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4499,7 +4499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -4885,8 +4885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y26" sqref="Y26"/>
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="AA43" sqref="AA43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9291,9 +9291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>